<commit_message>
shell scripts for model experiments
</commit_message>
<xml_diff>
--- a/references/Experiment_setup.xlsx
+++ b/references/Experiment_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\Master-Thesis\Fairness-oriented-interpretability-of-predictive-algorithms\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F374F28B-B89A-4013-AFB1-7F518E50C212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EA5451-7CD9-44C8-9F59-FA25A7A637E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{08E31009-6740-4219-8040-B32DB69AA2DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>Weight_decay</t>
   </si>
@@ -69,9 +69,6 @@
     <t>SGD</t>
   </si>
   <si>
-    <t>ADAM_wd_1e-2</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -81,36 +78,9 @@
     <t xml:space="preserve">Done </t>
   </si>
   <si>
-    <t>ADAM_wd_1e-3</t>
-  </si>
-  <si>
-    <t>ADAM_wd=1e-2_dp=0.1</t>
-  </si>
-  <si>
-    <t>ADAM_wd=0_dp=0.1</t>
-  </si>
-  <si>
-    <t>ADAM_wd=1e-2_dp=0.25</t>
-  </si>
-  <si>
-    <t>ADAM_wd=1e-3_dp=0.25</t>
-  </si>
-  <si>
-    <t>ADAM_wd=1e-3_dp=0.1</t>
-  </si>
-  <si>
-    <t>ADAM_wd=0_dp=0.25</t>
-  </si>
-  <si>
-    <t>Model_idx</t>
-  </si>
-  <si>
     <t>Parameter Options</t>
   </si>
   <si>
-    <t>ADAM_imgaug</t>
-  </si>
-  <si>
     <t>Extended ImgAug</t>
   </si>
   <si>
@@ -118,6 +88,69 @@
   </si>
   <si>
     <t>0.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh </t>
+  </si>
+  <si>
+    <t>adam_wd=1e-2</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-3</t>
+  </si>
+  <si>
+    <t>adam_dp=2e-1</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-2_dp=2e-1</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-3_dp=2e-1</t>
+  </si>
+  <si>
+    <t>adam_dp=4e-1</t>
+  </si>
+  <si>
+    <t>sh - on HPC</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-2_dp=4e-1</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-3_dp=4e-1</t>
+  </si>
+  <si>
+    <t>adam_imgaug</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-2_imgaug</t>
+  </si>
+  <si>
+    <t>adam_wd_1e-3_imgaug</t>
+  </si>
+  <si>
+    <t>adam_dp=2e-1_imgaug</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-2_dp=2e-1_imgaug</t>
+  </si>
+  <si>
+    <t>idx</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-3_dp=2e-1_imgaug</t>
+  </si>
+  <si>
+    <t>adam_dp=4e-1_imgaug</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-2_dp=4e-1_imgaug</t>
+  </si>
+  <si>
+    <t>adam_wd=1e-3_dp=4e-1_imgaug</t>
   </si>
 </sst>
 </file>
@@ -645,21 +678,22 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" customWidth="1"/>
+    <col min="2" max="2" width="28.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>5</v>
@@ -677,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M1" s="24"/>
     </row>
@@ -704,10 +738,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -737,7 +771,7 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>0</v>
@@ -758,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>K3</f>
@@ -775,6 +809,9 @@
       <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
       <c r="I4" s="14" t="s">
         <v>1</v>
       </c>
@@ -782,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="M4" s="24"/>
     </row>
@@ -794,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="str">
         <f>L3</f>
@@ -811,8 +848,11 @@
       <c r="F5" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
       <c r="I5" s="19" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J5" s="20" t="b">
         <v>1</v>
@@ -828,7 +868,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <f>J3</f>
@@ -845,13 +885,16 @@
       <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>K3</f>
@@ -868,13 +911,16 @@
       <c r="F7" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="str">
         <f>L3</f>
@@ -891,13 +937,16 @@
       <c r="F8" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1">
         <f>J3</f>
@@ -914,13 +963,16 @@
       <c r="F9" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>K3</f>
@@ -937,13 +989,16 @@
       <c r="F10" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C11" s="4" t="str">
         <f>L3</f>
@@ -960,13 +1015,16 @@
       <c r="F11" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1">
         <f>J3</f>
@@ -983,13 +1041,16 @@
       <c r="F12" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="str">
         <f>K3</f>
@@ -1006,13 +1067,16 @@
       <c r="F13" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>L3</f>
@@ -1029,20 +1093,23 @@
       <c r="F14" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1">
         <f>J3</f>
         <v>0</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E15" s="6" t="b">
         <f>J5</f>
@@ -1051,13 +1118,16 @@
       <c r="F15" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>K3</f>
@@ -1074,13 +1144,16 @@
       <c r="F16" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C17" s="4" t="str">
         <f>L3</f>
@@ -1097,13 +1170,16 @@
       <c r="F17" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1">
         <f>J3</f>
@@ -1120,13 +1196,16 @@
       <c r="F18" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3" t="str">
         <f>K3</f>
@@ -1143,13 +1222,16 @@
       <c r="F19" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>L3</f>
@@ -1165,6 +1247,9 @@
       </c>
       <c r="F20" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding initials to experiments
</commit_message>
<xml_diff>
--- a/references/Experiment_setup.xlsx
+++ b/references/Experiment_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\Master-Thesis\Fairness-oriented-interpretability-of-predictive-algorithms\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF7AFCD-DFA7-4874-94E5-5D16C2AE0029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EDE935-074C-41EE-9B83-0F2FB4BE39DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{08E31009-6740-4219-8040-B32DB69AA2DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>Weight_decay</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>HPC</t>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>EZ</t>
+  </si>
+  <si>
+    <t>CF</t>
   </si>
 </sst>
 </file>
@@ -681,7 +690,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,6 +725,9 @@
       <c r="G1" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="H1" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -742,6 +754,9 @@
       </c>
       <c r="G2" t="s">
         <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>14</v>
@@ -776,6 +791,9 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
       <c r="I3" s="14" t="s">
         <v>0</v>
       </c>
@@ -815,6 +833,9 @@
       <c r="G4" t="s">
         <v>38</v>
       </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
       <c r="I4" s="14" t="s">
         <v>1</v>
       </c>
@@ -854,6 +875,9 @@
       <c r="G5" t="s">
         <v>39</v>
       </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
       <c r="I5" s="19" t="s">
         <v>15</v>
       </c>
@@ -891,6 +915,9 @@
       <c r="G6" t="s">
         <v>39</v>
       </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -917,6 +944,9 @@
       <c r="G7" t="s">
         <v>39</v>
       </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -942,6 +972,9 @@
       </c>
       <c r="G8" t="s">
         <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>